<commit_message>
Fix SSH for CH + template til beregninger
</commit_message>
<xml_diff>
--- a/Data/Winrates_Data_2 - Kopi.xlsx
+++ b/Data/Winrates_Data_2 - Kopi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\speciale2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4D0B20-C2BD-44EE-ACFB-B3B766D28669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA57A6E-2170-4BD1-89F6-1CA60FC0CA27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B6D6821-1145-4596-9880-6E782CA02392}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Aggro DH</t>
   </si>
@@ -111,6 +111,48 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>L0</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Highlander hunter</t>
+  </si>
+  <si>
+    <t>Face</t>
+  </si>
+  <si>
+    <t>Pure P</t>
+  </si>
+  <si>
+    <t>Galak R</t>
+  </si>
+  <si>
+    <t>Control W</t>
+  </si>
+  <si>
+    <t>Gala Sha</t>
   </si>
 </sst>
 </file>
@@ -134,18 +176,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -195,16 +231,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,19 +626,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC015156-9DF1-4446-BEA9-1D9FD9389257}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.08984375" customWidth="1"/>
+    <col min="27" max="27" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D1">
         <f>1/COUNT($D$3:$W$3)</f>
         <v>0.05</v>
@@ -678,8 +722,29 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
+      <c r="Z1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -740,8 +805,29 @@
       <c r="W2" t="s">
         <v>19</v>
       </c>
+      <c r="Z2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -813,16 +899,42 @@
       <c r="W3" s="2">
         <v>34.979999999999997</v>
       </c>
-      <c r="X3">
-        <f>SUMPRODUCT(D3:W3,$D$26:$W$26)</f>
-        <v>51.354214285714278</v>
-      </c>
-      <c r="Y3">
-        <f>MAX(X3:X23)</f>
-        <v>53.323142857142855</v>
+      <c r="X3" s="12">
+        <f>SUM(D3:W3)*0.05*Z3+$AA$3*H3+$AB$3*G3+$AC$3*L3+$AD$3*O3+$AE$3*V3+Q3*$AF$3</f>
+        <v>63.029047813590097</v>
+      </c>
+      <c r="Y3" s="10">
+        <f>X3/SUM(X3:X23)</f>
+        <v>5.6528341541155533E-2</v>
+      </c>
+      <c r="Z3" s="8">
+        <f>4.21097904967754*10^(-15)</f>
+        <v>4.2109790496775403E-15</v>
+      </c>
+      <c r="AA3" s="8">
+        <f>31329.6841296009*10^(-16)</f>
+        <v>3.1329684129600902E-12</v>
+      </c>
+      <c r="AB3" s="8">
+        <f>1165464.24962115*10^(-15)</f>
+        <v>1.1654642496211502E-9</v>
+      </c>
+      <c r="AC3" s="8">
+        <f>289035133.906046*10^(-15)</f>
+        <v>2.8903513390604597E-7</v>
+      </c>
+      <c r="AD3" s="8">
+        <f>53760534906.5246*10^(-15)</f>
+        <v>5.3760534906524599E-5</v>
+      </c>
+      <c r="AE3" s="9">
+        <v>7.9995675940900193E-3</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>0.99194638166726801</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -867,7 +979,7 @@
       <c r="N4">
         <v>52.42</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>55.610000000000007</v>
       </c>
       <c r="P4">
@@ -894,12 +1006,13 @@
       <c r="W4">
         <v>58.52</v>
       </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X23" si="3">SUMPRODUCT(D4:W4,$D$26:$W$26)</f>
-        <v>41.254142857142845</v>
-      </c>
+      <c r="X4" s="12">
+        <f>SUM(D4:W4)*0.05*Z4+$AA$3*H4+$AB$3*G4+$AC$3*L4+$AD$3*O4+$AE$3*V4+Q4*$AF$3</f>
+        <v>42.217118958929262</v>
+      </c>
+      <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -971,12 +1084,13 @@
       <c r="W5">
         <v>48.480000000000004</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="3"/>
-        <v>44.192214285714279</v>
-      </c>
+      <c r="X5" s="12">
+        <f t="shared" ref="X5:X23" si="3">SUM(D5:W5)*0.05*Z5+$AA$3*H5+$AB$3*G5+$AC$3*L5+$AD$3*O5+$AE$3*V5+Q5*$AF$3</f>
+        <v>63.732973953506288</v>
+      </c>
+      <c r="Y5" s="10"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1048,12 +1162,13 @@
       <c r="W6">
         <v>51.76</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="13">
         <f t="shared" si="3"/>
-        <v>47.52757142857142</v>
-      </c>
+        <v>67.627564526019441</v>
+      </c>
+      <c r="Y6" s="11"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1125,12 +1240,17 @@
       <c r="W7">
         <v>50.580000000000005</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="12">
         <f t="shared" si="3"/>
-        <v>51.061571428571419</v>
+        <v>61.790653102103413</v>
+      </c>
+      <c r="Y7" s="10"/>
+      <c r="AA7">
+        <f>MAX(X3:X23)</f>
+        <v>67.632128544283006</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1202,12 +1322,13 @@
       <c r="W8">
         <v>60.12</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="12">
         <f t="shared" si="3"/>
-        <v>50.379428571428555</v>
-      </c>
+        <v>52.097741499385705</v>
+      </c>
+      <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1279,12 +1400,13 @@
       <c r="W9">
         <v>53.37</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="12">
         <f t="shared" si="3"/>
-        <v>43.992214285714276</v>
-      </c>
+        <v>45.788880332688414</v>
+      </c>
+      <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1356,12 +1478,17 @@
       <c r="W10">
         <v>36.309999999999995</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="13">
         <f t="shared" si="3"/>
-        <v>52.662499999999987</v>
+        <v>67.632128544283006</v>
+      </c>
+      <c r="Y10" s="11"/>
+      <c r="AA10">
+        <f>X6-X10</f>
+        <v>-4.5640182635651172E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1433,12 +1560,13 @@
       <c r="W11">
         <v>61.739999999999995</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="12">
         <f t="shared" si="3"/>
-        <v>51.514857142857139</v>
-      </c>
+        <v>55.165807355902508</v>
+      </c>
+      <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1510,12 +1638,13 @@
       <c r="W12">
         <v>71.17</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="12">
         <f t="shared" si="3"/>
-        <v>44.427714285714281</v>
-      </c>
+        <v>43.825191922433007</v>
+      </c>
+      <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1587,12 +1716,13 @@
       <c r="W13">
         <v>73.16</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="12">
         <f t="shared" si="3"/>
-        <v>43.720714285714287</v>
-      </c>
+        <v>45.605287814436267</v>
+      </c>
+      <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1664,12 +1794,13 @@
       <c r="W14">
         <v>46.949999999999996</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="12">
         <f t="shared" si="3"/>
-        <v>49.337285714285706</v>
-      </c>
+        <v>57.593353384456762</v>
+      </c>
+      <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1741,12 +1872,13 @@
       <c r="W15">
         <v>42.39</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="12">
         <f t="shared" si="3"/>
-        <v>44.982214285714278</v>
-      </c>
+        <v>43.756088655170338</v>
+      </c>
+      <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1818,12 +1950,13 @@
       <c r="W16">
         <v>58.69</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="12">
         <f t="shared" si="3"/>
-        <v>40.174857142857128</v>
-      </c>
+        <v>50.124297764525956</v>
+      </c>
+      <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1895,12 +2028,13 @@
       <c r="W17">
         <v>51.55</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="12">
         <f t="shared" si="3"/>
-        <v>40.499285714285705</v>
-      </c>
+        <v>44.272522978533786</v>
+      </c>
+      <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1972,12 +2106,13 @@
       <c r="W18">
         <v>35.480000000000004</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="12">
         <f t="shared" si="3"/>
-        <v>47.405999999999992</v>
-      </c>
+        <v>63.657113768191259</v>
+      </c>
+      <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2049,12 +2184,13 @@
       <c r="W19">
         <v>53.620000000000005</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="12">
         <f t="shared" si="3"/>
-        <v>52.416499999999985</v>
-      </c>
+        <v>58.344180944026114</v>
+      </c>
+      <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2126,12 +2262,13 @@
       <c r="W20">
         <v>45.12</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="12">
         <f t="shared" si="3"/>
-        <v>48.490500000000004</v>
-      </c>
+        <v>59.613757844874954</v>
+      </c>
+      <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2203,12 +2340,13 @@
       <c r="W21">
         <v>35.730000000000004</v>
       </c>
-      <c r="X21">
+      <c r="X21" s="12">
         <f t="shared" si="3"/>
-        <v>51.628785714285719</v>
-      </c>
+        <v>34.535857377691613</v>
+      </c>
+      <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2253,7 +2391,7 @@
       <c r="N22">
         <v>26.839999999999996</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="4">
         <v>53.05</v>
       </c>
       <c r="P22">
@@ -2280,12 +2418,13 @@
       <c r="W22" s="4">
         <v>50</v>
       </c>
-      <c r="X22">
+      <c r="X22" s="12">
         <f t="shared" si="3"/>
-        <v>53.323142857142855</v>
-      </c>
+        <v>41.494300347184847</v>
+      </c>
+      <c r="Y22" s="10"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D23">
         <f>SUMPRODUCT(D3:D22,$C$3:$C$22)</f>
         <v>50.753500000000003</v>
@@ -2366,12 +2505,13 @@
         <f t="shared" si="4"/>
         <v>50.986000000000004</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="12">
         <f t="shared" si="3"/>
-        <v>47.51728571428572</v>
-      </c>
+        <v>53.095193444396642</v>
+      </c>
+      <c r="Y23" s="10"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D25">
         <f>0.6*1/COUNT($D$3:$W$3)+D27*0.4</f>
         <v>0.03</v>
@@ -2453,7 +2593,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>21</v>
       </c>
@@ -2538,7 +2678,7 @@
         <v>2.1428571428571422E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>20</v>
       </c>
@@ -2603,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D30">
         <v>0</v>
       </c>
@@ -2616,7 +2756,7 @@
       <c r="G30">
         <v>3</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <v>4</v>
       </c>
       <c r="I30">
@@ -2625,10 +2765,10 @@
       <c r="J30">
         <v>6</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="6">
         <v>7</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="6">
         <v>8</v>
       </c>
       <c r="M30">
@@ -2661,11 +2801,11 @@
       <c r="V30">
         <v>18</v>
       </c>
-      <c r="W30" s="8">
+      <c r="W30" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G31" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Updates + CH model med mixed strats
</commit_message>
<xml_diff>
--- a/Data/Winrates_Data_2 - Kopi.xlsx
+++ b/Data/Winrates_Data_2 - Kopi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\speciale2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA57A6E-2170-4BD1-89F6-1CA60FC0CA27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9E1F8E-9F1F-440B-9CA2-C540651145DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B6D6821-1145-4596-9880-6E782CA02392}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Wooo CH model done
</commit_message>
<xml_diff>
--- a/Data/Winrates_Data_2 - Kopi.xlsx
+++ b/Data/Winrates_Data_2 - Kopi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\speciale2020\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9E1F8E-9F1F-440B-9CA2-C540651145DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F241FA8-2874-4FE1-AED2-0D768B65D552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B6D6821-1145-4596-9880-6E782CA02392}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Aggro DH</t>
   </si>
@@ -137,22 +137,28 @@
     <t>Mix</t>
   </si>
   <si>
-    <t>Highlander hunter</t>
-  </si>
-  <si>
-    <t>Face</t>
-  </si>
-  <si>
-    <t>Pure P</t>
-  </si>
-  <si>
-    <t>Galak R</t>
-  </si>
-  <si>
-    <t>Control W</t>
-  </si>
-  <si>
-    <t>Gala Sha</t>
+    <t>Enrage Warrior'</t>
+  </si>
+  <si>
+    <t>Highlander priest'</t>
+  </si>
+  <si>
+    <t>'Highlander Hunter', 'Quest warlock'</t>
+  </si>
+  <si>
+    <t>'Highlander priest', 'Galakrond shaman'</t>
+  </si>
+  <si>
+    <t>'Level-7 spiller: Totem shaman'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ['Highlander Hunter', 'Murloc Paladin']</t>
+  </si>
+  <si>
+    <t>Afrundet</t>
+  </si>
+  <si>
+    <t>Standard</t>
   </si>
 </sst>
 </file>
@@ -626,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC015156-9DF1-4446-BEA9-1D9FD9389257}">
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,11 +643,16 @@
     <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.08984375" customWidth="1"/>
-    <col min="27" max="27" width="16.08984375" customWidth="1"/>
+    <col min="24" max="26" width="11.08984375" customWidth="1"/>
+    <col min="28" max="28" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D1">
         <f>1/COUNT($D$3:$W$3)</f>
         <v>0.05</v>
@@ -722,29 +733,29 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -805,29 +816,38 @@
       <c r="W2" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="X2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
         <v>38</v>
       </c>
-      <c r="AF2" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -900,41 +920,45 @@
         <v>34.979999999999997</v>
       </c>
       <c r="X3" s="12">
-        <f>SUM(D3:W3)*0.05*Z3+$AA$3*H3+$AB$3*G3+$AC$3*L3+$AD$3*O3+$AE$3*V3+Q3*$AF$3</f>
+        <f>SUM(D3:W3)*0.05*AA3+$AB$3*H3+$AC$3*G3+$AD$3*L3+$AE$3*O3+$AF$3*V3+Q3*$AG$3</f>
         <v>63.029047813590097</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="12">
+        <f>SUM(D3:W3)*0.05*$AA$3+$AB$3*(H3+K3)/2+$AC$3*W3+$AD$3*N3+$AE$3*(H3+T3)/2+$AF$3*V3+$AG$3*(N3+Q3)/2</f>
+        <v>54.652213360723621</v>
+      </c>
+      <c r="Z3" s="10">
         <f>X3/SUM(X3:X23)</f>
         <v>5.6528341541155533E-2</v>
       </c>
-      <c r="Z3" s="8">
+      <c r="AA3" s="8">
         <f>4.21097904967754*10^(-15)</f>
         <v>4.2109790496775403E-15</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AB3" s="8">
         <f>31329.6841296009*10^(-16)</f>
         <v>3.1329684129600902E-12</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AC3" s="8">
         <f>1165464.24962115*10^(-15)</f>
         <v>1.1654642496211502E-9</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AD3" s="8">
         <f>289035133.906046*10^(-15)</f>
         <v>2.8903513390604597E-7</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AE3" s="8">
         <f>53760534906.5246*10^(-15)</f>
         <v>5.3760534906524599E-5</v>
       </c>
-      <c r="AE3" s="9">
+      <c r="AF3" s="9">
         <v>7.9995675940900193E-3</v>
       </c>
-      <c r="AF3" s="9">
+      <c r="AG3" s="9">
         <v>0.99194638166726801</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1007,12 +1031,16 @@
         <v>58.52</v>
       </c>
       <c r="X4" s="12">
-        <f>SUM(D4:W4)*0.05*Z4+$AA$3*H4+$AB$3*G4+$AC$3*L4+$AD$3*O4+$AE$3*V4+Q4*$AF$3</f>
+        <f>SUM(D4:W4)*0.05*AA4+$AB$3*H4+$AC$3*G4+$AD$3*L4+$AE$3*O4+$AF$3*V4+Q4*$AG$3</f>
         <v>42.217118958929262</v>
       </c>
-      <c r="Y4" s="10"/>
+      <c r="Y4" s="12">
+        <f t="shared" ref="Y4:Y23" si="3">SUM(D4:W4)*0.05*$AA$3+$AB$3*(H4+K4)/2+$AC$3*W4+$AD$3*N4+$AE$3*(H4+T4)/2+$AF$3*V4+$AG$3*(N4+Q4)/2</f>
+        <v>47.305457972155303</v>
+      </c>
+      <c r="Z4" s="10"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1085,12 +1113,16 @@
         <v>48.480000000000004</v>
       </c>
       <c r="X5" s="12">
-        <f t="shared" ref="X5:X23" si="3">SUM(D5:W5)*0.05*Z5+$AA$3*H5+$AB$3*G5+$AC$3*L5+$AD$3*O5+$AE$3*V5+Q5*$AF$3</f>
+        <f t="shared" ref="X5:X23" si="4">SUM(D5:W5)*0.05*AA5+$AB$3*H5+$AC$3*G5+$AD$3*L5+$AE$3*O5+$AF$3*V5+Q5*$AG$3</f>
         <v>63.732973953506288</v>
       </c>
-      <c r="Y5" s="10"/>
+      <c r="Y5" s="12">
+        <f t="shared" si="3"/>
+        <v>58.897606683814132</v>
+      </c>
+      <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1163,12 +1195,16 @@
         <v>51.76</v>
       </c>
       <c r="X6" s="13">
+        <f t="shared" si="4"/>
+        <v>67.627564526019441</v>
+      </c>
+      <c r="Y6" s="12">
         <f t="shared" si="3"/>
-        <v>67.627564526019441</v>
-      </c>
-      <c r="Y6" s="11"/>
+        <v>53.661243118790509</v>
+      </c>
+      <c r="Z6" s="11"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1241,16 +1277,20 @@
         <v>50.580000000000005</v>
       </c>
       <c r="X7" s="12">
+        <f t="shared" si="4"/>
+        <v>61.790653102103413</v>
+      </c>
+      <c r="Y7" s="13">
         <f t="shared" si="3"/>
-        <v>61.790653102103413</v>
-      </c>
-      <c r="Y7" s="10"/>
-      <c r="AA7">
+        <v>62.256775636409792</v>
+      </c>
+      <c r="Z7" s="10"/>
+      <c r="AB7">
         <f>MAX(X3:X23)</f>
         <v>67.632128544283006</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1323,12 +1363,16 @@
         <v>60.12</v>
       </c>
       <c r="X8" s="12">
+        <f t="shared" si="4"/>
+        <v>52.097741499385705</v>
+      </c>
+      <c r="Y8" s="12">
         <f t="shared" si="3"/>
-        <v>52.097741499385705</v>
-      </c>
-      <c r="Y8" s="10"/>
+        <v>54.428298375850268</v>
+      </c>
+      <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1401,12 +1445,16 @@
         <v>53.37</v>
       </c>
       <c r="X9" s="12">
+        <f t="shared" si="4"/>
+        <v>45.788880332688414</v>
+      </c>
+      <c r="Y9" s="12">
         <f t="shared" si="3"/>
-        <v>45.788880332688414</v>
-      </c>
-      <c r="Y9" s="10"/>
+        <v>47.445047644787941</v>
+      </c>
+      <c r="Z9" s="10"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1479,16 +1527,20 @@
         <v>36.309999999999995</v>
       </c>
       <c r="X10" s="13">
+        <f t="shared" si="4"/>
+        <v>67.632128544283006</v>
+      </c>
+      <c r="Y10" s="12">
         <f t="shared" si="3"/>
-        <v>67.632128544283006</v>
-      </c>
-      <c r="Y10" s="11"/>
-      <c r="AA10">
+        <v>62.414274181220442</v>
+      </c>
+      <c r="Z10" s="11"/>
+      <c r="AB10">
         <f>X6-X10</f>
         <v>-4.5640182635651172E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1561,12 +1613,16 @@
         <v>61.739999999999995</v>
       </c>
       <c r="X11" s="12">
+        <f t="shared" si="4"/>
+        <v>55.165807355902508</v>
+      </c>
+      <c r="Y11" s="12">
         <f t="shared" si="3"/>
-        <v>55.165807355902508</v>
-      </c>
-      <c r="Y11" s="10"/>
+        <v>50.469677868448507</v>
+      </c>
+      <c r="Z11" s="10"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1639,12 +1695,16 @@
         <v>71.17</v>
       </c>
       <c r="X12" s="12">
+        <f t="shared" si="4"/>
+        <v>43.825191922433007</v>
+      </c>
+      <c r="Y12" s="12">
         <f t="shared" si="3"/>
-        <v>43.825191922433007</v>
-      </c>
-      <c r="Y12" s="10"/>
+        <v>49.954854046634864</v>
+      </c>
+      <c r="Z12" s="10"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1717,12 +1777,16 @@
         <v>73.16</v>
       </c>
       <c r="X13" s="12">
+        <f t="shared" si="4"/>
+        <v>45.605287814436267</v>
+      </c>
+      <c r="Y13" s="12">
         <f t="shared" si="3"/>
-        <v>45.605287814436267</v>
-      </c>
-      <c r="Y13" s="10"/>
+        <v>47.861752004942268</v>
+      </c>
+      <c r="Z13" s="10"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1795,12 +1859,16 @@
         <v>46.949999999999996</v>
       </c>
       <c r="X14" s="12">
+        <f t="shared" si="4"/>
+        <v>57.593353384456762</v>
+      </c>
+      <c r="Y14" s="12">
         <f t="shared" si="3"/>
-        <v>57.593353384456762</v>
-      </c>
-      <c r="Y14" s="10"/>
+        <v>58.118882329130287</v>
+      </c>
+      <c r="Z14" s="10"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1873,12 +1941,16 @@
         <v>42.39</v>
       </c>
       <c r="X15" s="12">
+        <f t="shared" si="4"/>
+        <v>43.756088655170338</v>
+      </c>
+      <c r="Y15" s="12">
         <f t="shared" si="3"/>
-        <v>43.756088655170338</v>
-      </c>
-      <c r="Y15" s="10"/>
+        <v>49.16707023195864</v>
+      </c>
+      <c r="Z15" s="10"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1951,12 +2023,16 @@
         <v>58.69</v>
       </c>
       <c r="X16" s="12">
+        <f t="shared" si="4"/>
+        <v>50.124297764525956</v>
+      </c>
+      <c r="Y16" s="12">
         <f t="shared" si="3"/>
-        <v>50.124297764525956</v>
-      </c>
-      <c r="Y16" s="10"/>
+        <v>52.380843169609363</v>
+      </c>
+      <c r="Z16" s="10"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2029,12 +2105,16 @@
         <v>51.55</v>
       </c>
       <c r="X17" s="12">
+        <f t="shared" si="4"/>
+        <v>44.272522978533786</v>
+      </c>
+      <c r="Y17" s="12">
         <f t="shared" si="3"/>
-        <v>44.272522978533786</v>
-      </c>
-      <c r="Y17" s="10"/>
+        <v>44.207744592819019</v>
+      </c>
+      <c r="Z17" s="10"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2107,12 +2187,16 @@
         <v>35.480000000000004</v>
       </c>
       <c r="X18" s="12">
+        <f t="shared" si="4"/>
+        <v>63.657113768191259</v>
+      </c>
+      <c r="Y18" s="13">
         <f t="shared" si="3"/>
-        <v>63.657113768191259</v>
-      </c>
-      <c r="Y18" s="10"/>
+        <v>62.863814092998972</v>
+      </c>
+      <c r="Z18" s="10"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2185,12 +2269,16 @@
         <v>53.620000000000005</v>
       </c>
       <c r="X19" s="12">
+        <f t="shared" si="4"/>
+        <v>58.344180944026114</v>
+      </c>
+      <c r="Y19" s="12">
         <f t="shared" si="3"/>
-        <v>58.344180944026114</v>
-      </c>
-      <c r="Y19" s="10"/>
+        <v>60.352569601185522</v>
+      </c>
+      <c r="Z19" s="10"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2263,12 +2351,16 @@
         <v>45.12</v>
       </c>
       <c r="X20" s="12">
+        <f t="shared" si="4"/>
+        <v>59.613757844874954</v>
+      </c>
+      <c r="Y20" s="12">
         <f t="shared" si="3"/>
-        <v>59.613757844874954</v>
-      </c>
-      <c r="Y20" s="10"/>
+        <v>57.545415909068339</v>
+      </c>
+      <c r="Z20" s="10"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2341,12 +2433,16 @@
         <v>35.730000000000004</v>
       </c>
       <c r="X21" s="12">
+        <f t="shared" si="4"/>
+        <v>34.535857377691613</v>
+      </c>
+      <c r="Y21" s="12">
         <f t="shared" si="3"/>
-        <v>34.535857377691613</v>
-      </c>
-      <c r="Y21" s="10"/>
+        <v>34.883206453344592</v>
+      </c>
+      <c r="Z21" s="10"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2419,181 +2515,189 @@
         <v>50</v>
       </c>
       <c r="X22" s="12">
+        <f t="shared" si="4"/>
+        <v>41.494300347184847</v>
+      </c>
+      <c r="Y22" s="12">
         <f t="shared" si="3"/>
-        <v>41.494300347184847</v>
-      </c>
-      <c r="Y22" s="10"/>
+        <v>34.317288110359947</v>
+      </c>
+      <c r="Z22" s="10"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D23">
         <f>SUMPRODUCT(D3:D22,$C$3:$C$22)</f>
         <v>50.753500000000003</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:W23" si="4">SUMPRODUCT(E3:E22,$C$3:$C$22)</f>
+        <f t="shared" ref="E23:W23" si="5">SUMPRODUCT(E3:E22,$C$3:$C$22)</f>
         <v>53.207000000000008</v>
       </c>
       <c r="F23">
+        <f t="shared" si="5"/>
+        <v>48.331500000000013</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>48.009</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="5"/>
+        <v>45.563000000000002</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>47.328000000000003</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>51.63150000000001</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>45.747500000000002</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="5"/>
+        <v>47.212000000000003</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="5"/>
+        <v>50.621999999999993</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>51.244999999999997</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="5"/>
+        <v>48.913000000000011</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="5"/>
+        <v>53.761499999999998</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>53.131999999999998</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="5"/>
+        <v>58.25500000000001</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="5"/>
+        <v>47.785999999999994</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="5"/>
+        <v>48.861500000000007</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="5"/>
+        <v>50.095500000000001</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="5"/>
+        <v>48.559500000000007</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="5"/>
+        <v>50.986000000000004</v>
+      </c>
+      <c r="X23" s="12">
         <f t="shared" si="4"/>
-        <v>48.331500000000013</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>48.009</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>45.563000000000002</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="4"/>
-        <v>47.328000000000003</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="4"/>
-        <v>51.63150000000001</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="4"/>
-        <v>45.747500000000002</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="4"/>
-        <v>47.212000000000003</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="4"/>
-        <v>50.621999999999993</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="4"/>
-        <v>51.244999999999997</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="4"/>
-        <v>48.913000000000011</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="4"/>
-        <v>53.761499999999998</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>53.131999999999998</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="4"/>
-        <v>58.25500000000001</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="4"/>
-        <v>47.785999999999994</v>
-      </c>
-      <c r="T23">
-        <f t="shared" si="4"/>
-        <v>48.861500000000007</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="4"/>
-        <v>50.095500000000001</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="4"/>
-        <v>48.559500000000007</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="4"/>
-        <v>50.986000000000004</v>
-      </c>
-      <c r="X23" s="12">
+        <v>53.095193444396642</v>
+      </c>
+      <c r="Y23" s="12">
         <f t="shared" si="3"/>
-        <v>53.095193444396642</v>
-      </c>
-      <c r="Y23" s="10"/>
+        <v>52.159201769212615</v>
+      </c>
+      <c r="Z23" s="10"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D25">
         <f>0.6*1/COUNT($D$3:$W$3)+D27*0.4</f>
         <v>0.03</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:W25" si="5">0.6*1/COUNT($D$3:$W$3)+E27*0.4</f>
+        <f t="shared" ref="E25:W25" si="6">0.6*1/COUNT($D$3:$W$3)+E27*0.4</f>
         <v>0.03</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.43000000000000005</v>
       </c>
       <c r="I25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="J25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="K25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.43000000000000005</v>
       </c>
       <c r="L25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="M25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="N25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="O25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="P25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="R25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="S25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="T25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="U25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="V25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
       <c r="W25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>21</v>
       </c>
@@ -2602,83 +2706,83 @@
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26:W26" si="6">E25/SUM($D$25:$W$25)</f>
+        <f t="shared" ref="E26:W26" si="7">E25/SUM($D$25:$W$25)</f>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="G26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30714285714285711</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="J26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30714285714285711</v>
       </c>
       <c r="L26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="M26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="O26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="R26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="S26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="T26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="U26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="V26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
       <c r="W26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1428571428571422E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>20</v>
       </c>
@@ -2743,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D30">
         <v>0</v>
       </c>
@@ -2805,7 +2909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="G31" t="s">
         <v>22</v>
       </c>

</xml_diff>